<commit_message>
Started uploading excel tutorials
</commit_message>
<xml_diff>
--- a/docs/distributions/normal_z_scores_percentages.xlsx
+++ b/docs/distributions/normal_z_scores_percentages.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nt906822/Documents/github/reading-psych/jast/distributions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F80169-6A17-AA4F-93BD-A9AAD33DC9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741FD69-00B1-B844-8BC2-B243FAF2D867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{B6F779AA-201C-5540-AA47-08BAC5B44788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,7 +65,7 @@
     <t>84.1% to 97.7%</t>
   </si>
   <si>
-    <t>97% to 100%</t>
+    <t>97.7% to 100%</t>
   </si>
 </sst>
 </file>
@@ -1709,513 +1706,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>frequency</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>120</v>
-          </cell>
-          <cell r="B2">
-            <v>4.4318484119380098E-4</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>121</v>
-          </cell>
-          <cell r="B3">
-            <v>5.9525324197758501E-4</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>122</v>
-          </cell>
-          <cell r="B4">
-            <v>7.9154515829799705E-4</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>123</v>
-          </cell>
-          <cell r="B5">
-            <v>1.04209348144226E-3</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>124</v>
-          </cell>
-          <cell r="B6">
-            <v>1.3582969233685599E-3</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>125</v>
-          </cell>
-          <cell r="B7">
-            <v>1.7528300493568499E-3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>126</v>
-          </cell>
-          <cell r="B8">
-            <v>2.2394530294842902E-3</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>127</v>
-          </cell>
-          <cell r="B9">
-            <v>2.8327037741601199E-3</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>128</v>
-          </cell>
-          <cell r="B10">
-            <v>3.5474592846231399E-3</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>129</v>
-          </cell>
-          <cell r="B11">
-            <v>4.3983595980427196E-3</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>130</v>
-          </cell>
-          <cell r="B12">
-            <v>5.3990966513188096E-3</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>131</v>
-          </cell>
-          <cell r="B13">
-            <v>6.5615814774676604E-3</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>132</v>
-          </cell>
-          <cell r="B14">
-            <v>7.8950158300894208E-3</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>133</v>
-          </cell>
-          <cell r="B15">
-            <v>9.4049077376887006E-3</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>134</v>
-          </cell>
-          <cell r="B16">
-            <v>1.10920834679456E-2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>135</v>
-          </cell>
-          <cell r="B17">
-            <v>1.2951759566589199E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>136</v>
-          </cell>
-          <cell r="B18">
-            <v>1.49727465635745E-2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>137</v>
-          </cell>
-          <cell r="B19">
-            <v>1.71368592047807E-2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>138</v>
-          </cell>
-          <cell r="B20">
-            <v>1.9418605498321299E-2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>139</v>
-          </cell>
-          <cell r="B21">
-            <v>2.1785217703255099E-2</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>140</v>
-          </cell>
-          <cell r="B22">
-            <v>2.4197072451914301E-2</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>141</v>
-          </cell>
-          <cell r="B23">
-            <v>2.6608524989875499E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>142</v>
-          </cell>
-          <cell r="B24">
-            <v>2.8969155276148299E-2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>143</v>
-          </cell>
-          <cell r="B25">
-            <v>3.1225393336676101E-2</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>144</v>
-          </cell>
-          <cell r="B26">
-            <v>3.3322460289179998E-2</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>145</v>
-          </cell>
-          <cell r="B27">
-            <v>3.5206532676430001E-2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>146</v>
-          </cell>
-          <cell r="B28">
-            <v>3.6827014030332297E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>147</v>
-          </cell>
-          <cell r="B29">
-            <v>3.8138781546052401E-2</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>148</v>
-          </cell>
-          <cell r="B30">
-            <v>3.9104269397545598E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>149</v>
-          </cell>
-          <cell r="B31">
-            <v>3.9695254747701199E-2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>150</v>
-          </cell>
-          <cell r="B32">
-            <v>3.9894228040143302E-2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>151</v>
-          </cell>
-          <cell r="B33">
-            <v>3.9695254747701199E-2</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>152</v>
-          </cell>
-          <cell r="B34">
-            <v>3.9104269397545598E-2</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>153</v>
-          </cell>
-          <cell r="B35">
-            <v>3.8138781546052401E-2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>154</v>
-          </cell>
-          <cell r="B36">
-            <v>3.6827014030332297E-2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>155</v>
-          </cell>
-          <cell r="B37">
-            <v>3.5206532676430001E-2</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>156</v>
-          </cell>
-          <cell r="B38">
-            <v>3.3322460289179998E-2</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>157</v>
-          </cell>
-          <cell r="B39">
-            <v>3.1225393336676101E-2</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>158</v>
-          </cell>
-          <cell r="B40">
-            <v>2.8969155276148299E-2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>159</v>
-          </cell>
-          <cell r="B41">
-            <v>2.6608524989875499E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>160</v>
-          </cell>
-          <cell r="B42">
-            <v>2.4197072451914301E-2</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>161</v>
-          </cell>
-          <cell r="B43">
-            <v>2.1785217703255099E-2</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>162</v>
-          </cell>
-          <cell r="B44">
-            <v>1.9418605498321299E-2</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>163</v>
-          </cell>
-          <cell r="B45">
-            <v>1.71368592047807E-2</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>164</v>
-          </cell>
-          <cell r="B46">
-            <v>1.49727465635745E-2</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>165</v>
-          </cell>
-          <cell r="B47">
-            <v>1.2951759566589199E-2</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>166</v>
-          </cell>
-          <cell r="B48">
-            <v>1.10920834679456E-2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>167</v>
-          </cell>
-          <cell r="B49">
-            <v>9.4049077376887006E-3</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>168</v>
-          </cell>
-          <cell r="B50">
-            <v>7.8950158300894208E-3</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51">
-            <v>169</v>
-          </cell>
-          <cell r="B51">
-            <v>6.5615814774676604E-3</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52">
-            <v>170</v>
-          </cell>
-          <cell r="B52">
-            <v>5.3990966513188096E-3</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>171</v>
-          </cell>
-          <cell r="B53">
-            <v>4.3983595980427196E-3</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>172</v>
-          </cell>
-          <cell r="B54">
-            <v>3.5474592846231399E-3</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>173</v>
-          </cell>
-          <cell r="B55">
-            <v>2.8327037741601199E-3</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>174</v>
-          </cell>
-          <cell r="B56">
-            <v>2.2394530294842902E-3</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57">
-            <v>175</v>
-          </cell>
-          <cell r="B57">
-            <v>1.7528300493568499E-3</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58">
-            <v>176</v>
-          </cell>
-          <cell r="B58">
-            <v>1.3582969233685599E-3</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59">
-            <v>177</v>
-          </cell>
-          <cell r="B59">
-            <v>1.04209348144226E-3</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60">
-            <v>178</v>
-          </cell>
-          <cell r="B60">
-            <v>7.9154515829799705E-4</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61">
-            <v>179</v>
-          </cell>
-          <cell r="B61">
-            <v>5.9525324197758501E-4</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62">
-            <v>180</v>
-          </cell>
-          <cell r="B62">
-            <v>4.4318484119380098E-4</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2516,7 +2006,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2546,7 +2036,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <f>(A2-AVERAGE(A:A))/10</f>
+        <f t="shared" ref="C2:C33" si="0">(A2-AVERAGE(A:A))/10</f>
         <v>-3</v>
       </c>
       <c r="D2">
@@ -2561,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f>(A3-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.9</v>
       </c>
       <c r="D3">
@@ -2576,7 +2066,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <f>(A4-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.8</v>
       </c>
       <c r="D4">
@@ -2591,7 +2081,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f>(A5-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.7</v>
       </c>
       <c r="D5">
@@ -2606,7 +2096,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <f>(A6-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.6</v>
       </c>
       <c r="D6">
@@ -2621,7 +2111,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f>(A7-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.5</v>
       </c>
       <c r="D7">
@@ -2636,7 +2126,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <f>(A8-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.4</v>
       </c>
       <c r="D8">
@@ -2651,7 +2141,7 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <f>(A9-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.2999999999999998</v>
       </c>
       <c r="D9">
@@ -2666,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <f>(A10-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.2000000000000002</v>
       </c>
       <c r="D10">
@@ -2681,7 +2171,7 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <f>(A11-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2.1</v>
       </c>
       <c r="D11">
@@ -2696,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <f>(A12-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="D12">
@@ -2711,7 +2201,7 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <f>(A13-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.9</v>
       </c>
       <c r="D13">
@@ -2726,7 +2216,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <f>(A14-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.8</v>
       </c>
       <c r="D14">
@@ -2741,7 +2231,7 @@
         <v>5</v>
       </c>
       <c r="C15">
-        <f>(A15-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.7</v>
       </c>
       <c r="D15">
@@ -2756,7 +2246,7 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <f>(A16-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.6</v>
       </c>
       <c r="D16">
@@ -2771,7 +2261,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <f>(A17-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.5</v>
       </c>
       <c r="D17">
@@ -2786,7 +2276,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <f>(A18-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.4</v>
       </c>
       <c r="D18">
@@ -2801,7 +2291,7 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <f>(A19-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.3</v>
       </c>
       <c r="D19">
@@ -2816,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <f>(A20-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.2</v>
       </c>
       <c r="D20">
@@ -2831,7 +2321,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <f>(A21-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1.1000000000000001</v>
       </c>
       <c r="D21">
@@ -2846,7 +2336,7 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <f>(A22-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="D22">
@@ -2861,7 +2351,7 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <f>(A23-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.9</v>
       </c>
       <c r="D23">
@@ -2876,7 +2366,7 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <f>(A24-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.8</v>
       </c>
       <c r="D24">
@@ -2891,7 +2381,7 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <f>(A25-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.7</v>
       </c>
       <c r="D25">
@@ -2906,7 +2396,7 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <f>(A26-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.6</v>
       </c>
       <c r="D26">
@@ -2921,7 +2411,7 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <f>(A27-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
       <c r="D27">
@@ -2936,7 +2426,7 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <f>(A28-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.4</v>
       </c>
       <c r="D28">
@@ -2951,7 +2441,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <f>(A29-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.3</v>
       </c>
       <c r="D29">
@@ -2966,7 +2456,7 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <f>(A30-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.2</v>
       </c>
       <c r="D30">
@@ -2981,7 +2471,7 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <f>(A31-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>-0.1</v>
       </c>
       <c r="D31">
@@ -2996,7 +2486,7 @@
         <v>7</v>
       </c>
       <c r="C32">
-        <f>(A32-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D32">
@@ -3011,7 +2501,7 @@
         <v>7</v>
       </c>
       <c r="C33">
-        <f>(A33-AVERAGE(A:A))/10</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="D33">
@@ -3026,7 +2516,7 @@
         <v>7</v>
       </c>
       <c r="C34">
-        <f>(A34-AVERAGE(A:A))/10</f>
+        <f t="shared" ref="C34:C62" si="1">(A34-AVERAGE(A:A))/10</f>
         <v>0.2</v>
       </c>
       <c r="D34">
@@ -3041,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="C35">
-        <f>(A35-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="D35">
@@ -3056,7 +2546,7 @@
         <v>7</v>
       </c>
       <c r="C36">
-        <f>(A36-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="D36">
@@ -3071,7 +2561,7 @@
         <v>7</v>
       </c>
       <c r="C37">
-        <f>(A37-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="D37">
@@ -3086,7 +2576,7 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <f>(A38-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="D38">
@@ -3101,7 +2591,7 @@
         <v>7</v>
       </c>
       <c r="C39">
-        <f>(A39-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="D39">
@@ -3116,7 +2606,7 @@
         <v>7</v>
       </c>
       <c r="C40">
-        <f>(A40-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="D40">
@@ -3131,7 +2621,7 @@
         <v>7</v>
       </c>
       <c r="C41">
-        <f>(A41-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
       <c r="D41">
@@ -3146,7 +2636,7 @@
         <v>8</v>
       </c>
       <c r="C42">
-        <f>(A42-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D42">
@@ -3161,7 +2651,7 @@
         <v>8</v>
       </c>
       <c r="C43">
-        <f>(A43-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="D43">
@@ -3176,7 +2666,7 @@
         <v>8</v>
       </c>
       <c r="C44">
-        <f>(A44-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="D44">
@@ -3191,7 +2681,7 @@
         <v>8</v>
       </c>
       <c r="C45">
-        <f>(A45-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
       <c r="D45">
@@ -3206,7 +2696,7 @@
         <v>8</v>
       </c>
       <c r="C46">
-        <f>(A46-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
       <c r="D46">
@@ -3221,7 +2711,7 @@
         <v>8</v>
       </c>
       <c r="C47">
-        <f>(A47-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="D47">
@@ -3236,7 +2726,7 @@
         <v>8</v>
       </c>
       <c r="C48">
-        <f>(A48-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="D48">
@@ -3251,7 +2741,7 @@
         <v>8</v>
       </c>
       <c r="C49">
-        <f>(A49-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.7</v>
       </c>
       <c r="D49">
@@ -3266,7 +2756,7 @@
         <v>8</v>
       </c>
       <c r="C50">
-        <f>(A50-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
       <c r="D50">
@@ -3281,7 +2771,7 @@
         <v>8</v>
       </c>
       <c r="C51">
-        <f>(A51-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
       <c r="D51">
@@ -3296,7 +2786,7 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <f>(A52-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D52">
@@ -3311,7 +2801,7 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <f>(A53-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="D53">
@@ -3326,7 +2816,7 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <f>(A54-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="D54">
@@ -3341,7 +2831,7 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <f>(A55-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="D55">
@@ -3356,7 +2846,7 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <f>(A56-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
       <c r="D56">
@@ -3371,7 +2861,7 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <f>(A57-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="D57">
@@ -3386,7 +2876,7 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <f>(A58-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
       <c r="D58">
@@ -3401,7 +2891,7 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <f>(A59-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.7</v>
       </c>
       <c r="D59">
@@ -3416,7 +2906,7 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <f>(A60-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="D60">
@@ -3431,7 +2921,7 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <f>(A61-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>2.9</v>
       </c>
       <c r="D61">
@@ -3446,7 +2936,7 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <f>(A62-AVERAGE(A:A))/10</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D62">

</xml_diff>